<commit_message>
Add short check to Prototype BOM
git-svn-id: https://svn.ee.ethz.ch/tecdoc/sigristl/projects/RocketLogger@38410 087458d4-8f0a-0410-b608-9ee62c3558fa
</commit_message>
<xml_diff>
--- a/code/pcb/Cape/Project Outputs for Cape/BOM/Bill of Materials-Cape-Prototype.xlsx
+++ b/code/pcb/Cape/Project Outputs for Cape/BOM/Bill of Materials-Cape-Prototype.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="718">
   <si>
     <t>Qty</t>
   </si>
@@ -2162,6 +2162,12 @@
   </si>
   <si>
     <t>replaced with 1276-1100-1-ND</t>
+  </si>
+  <si>
+    <t>Number of lines</t>
+  </si>
+  <si>
+    <t>Total cost</t>
   </si>
 </sst>
 </file>
@@ -2659,12 +2665,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3007,10 +3014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG87"/>
+  <dimension ref="A1:AG89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="AG13" sqref="AG13"/>
+    <sheetView tabSelected="1" topLeftCell="K62" workbookViewId="0">
+      <selection activeCell="AA87" sqref="AA87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10849,9 +10856,21 @@
       </c>
     </row>
     <row r="87" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AA87" s="5" t="s">
+        <v>717</v>
+      </c>
       <c r="AC87" s="4">
         <f>SUM(AC3:AC86)</f>
         <v>57.737641093999876</v>
+      </c>
+    </row>
+    <row r="89" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AA89" s="5" t="s">
+        <v>716</v>
+      </c>
+      <c r="AC89">
+        <f>COUNTIF(AC3:AC85,"&gt;0")</f>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>